<commit_message>
A range of updates to nutrientCalcs.R for cleanup. For example, replaced the 'commodity' column name with 'IMPACT_code' because that's what these are.
</commit_message>
<xml_diff>
--- a/data/DRI EAR values.xlsx
+++ b/data/DRI EAR values.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27580" yWindow="-3500" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DRI -RDA&amp;AI" sheetId="2" r:id="rId1"/>
@@ -347,6 +347,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -360,12 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -714,44 +714,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" s="3" customFormat="1" ht="13">
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="21" t="s">
+      <c r="F1" s="24"/>
+      <c r="G1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="18" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="18" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="18" t="s">
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:96" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -853,8 +856,8 @@
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
-      <c r="BO2" s="24"/>
-      <c r="BP2" s="24"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
       <c r="BQ2" s="15"/>
       <c r="BR2" s="15"/>
       <c r="BS2" s="15"/>
@@ -885,9 +888,6 @@
       <c r="CR2" s="15"/>
     </row>
     <row r="3" spans="1:96">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1253,8 +1253,8 @@
       <c r="BL5" s="8"/>
       <c r="BM5" s="8"/>
       <c r="BN5" s="3"/>
-      <c r="BO5" s="23"/>
-      <c r="BP5" s="23"/>
+      <c r="BO5" s="18"/>
+      <c r="BP5" s="18"/>
       <c r="BR5" s="5"/>
       <c r="BS5" s="5"/>
       <c r="BU5" s="5"/>
@@ -3795,8 +3795,8 @@
       <c r="BL37" s="9"/>
       <c r="BM37" s="9"/>
       <c r="BN37" s="3"/>
-      <c r="BO37" s="23"/>
-      <c r="BP37" s="23"/>
+      <c r="BO37" s="18"/>
+      <c r="BP37" s="18"/>
       <c r="BR37" s="5"/>
       <c r="BS37" s="5"/>
       <c r="BU37" s="8"/>
@@ -4042,8 +4042,8 @@
       <c r="BK40" s="8"/>
       <c r="BL40" s="8"/>
       <c r="BM40" s="8"/>
-      <c r="BO40" s="23"/>
-      <c r="BP40" s="23"/>
+      <c r="BO40" s="18"/>
+      <c r="BP40" s="18"/>
       <c r="BR40" s="5"/>
       <c r="BS40" s="5"/>
       <c r="BU40" s="5"/>
@@ -4313,8 +4313,8 @@
       <c r="BK43" s="11"/>
       <c r="BL43" s="11"/>
       <c r="BM43" s="11"/>
-      <c r="BO43" s="23"/>
-      <c r="BP43" s="23"/>
+      <c r="BO43" s="18"/>
+      <c r="BP43" s="18"/>
       <c r="BR43" s="5"/>
       <c r="BS43" s="5"/>
       <c r="BU43" s="8"/>
@@ -4388,8 +4388,8 @@
       <c r="BK44" s="8"/>
       <c r="BL44" s="8"/>
       <c r="BM44" s="8"/>
-      <c r="BO44" s="23"/>
-      <c r="BP44" s="23"/>
+      <c r="BO44" s="18"/>
+      <c r="BP44" s="18"/>
       <c r="BR44" s="5"/>
       <c r="BS44" s="5"/>
       <c r="BU44" s="5"/>
@@ -4463,8 +4463,8 @@
       <c r="BK45" s="11"/>
       <c r="BL45" s="11"/>
       <c r="BM45" s="11"/>
-      <c r="BO45" s="23"/>
-      <c r="BP45" s="23"/>
+      <c r="BO45" s="18"/>
+      <c r="BP45" s="18"/>
       <c r="BR45" s="5"/>
       <c r="BS45" s="5"/>
       <c r="BU45" s="8"/>
@@ -4538,8 +4538,8 @@
       <c r="BK46" s="8"/>
       <c r="BL46" s="8"/>
       <c r="BM46" s="8"/>
-      <c r="BO46" s="23"/>
-      <c r="BP46" s="23"/>
+      <c r="BO46" s="18"/>
+      <c r="BP46" s="18"/>
       <c r="BR46" s="5"/>
       <c r="BS46" s="5"/>
       <c r="BU46" s="8"/>
@@ -4613,8 +4613,8 @@
       <c r="BK47" s="11"/>
       <c r="BL47" s="11"/>
       <c r="BM47" s="11"/>
-      <c r="BO47" s="23"/>
-      <c r="BP47" s="23"/>
+      <c r="BO47" s="18"/>
+      <c r="BP47" s="18"/>
       <c r="BR47" s="5"/>
       <c r="BS47" s="5"/>
       <c r="BU47" s="8"/>
@@ -4763,8 +4763,8 @@
       <c r="BK49" s="4"/>
       <c r="BL49" s="4"/>
       <c r="BM49" s="4"/>
-      <c r="BO49" s="23"/>
-      <c r="BP49" s="23"/>
+      <c r="BO49" s="18"/>
+      <c r="BP49" s="18"/>
       <c r="BR49" s="5"/>
       <c r="BS49" s="5"/>
       <c r="BU49" s="5"/>
@@ -5079,6 +5079,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="BO45:BP45"/>
     <mergeCell ref="BO46:BP46"/>
     <mergeCell ref="BO47:BP47"/>
@@ -5089,12 +5095,6 @@
     <mergeCell ref="BO40:BP40"/>
     <mergeCell ref="BO43:BP43"/>
     <mergeCell ref="BO44:BP44"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>